<commit_message>
Combination area chart template
</commit_message>
<xml_diff>
--- a/Merck Sereno Dashboard/Dashboard/Content/ExportTemplate/CombinationAreaChart.xlsx
+++ b/Merck Sereno Dashboard/Dashboard/Content/ExportTemplate/CombinationAreaChart.xlsx
@@ -15,8 +15,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -56,9 +64,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -108,8 +117,8 @@
           <c:yMode val="edge"/>
           <c:x val="5.0623120491736791E-2"/>
           <c:y val="6.6470669494486559E-2"/>
-          <c:w val="0.82367936243671447"/>
-          <c:h val="0.8507567668592505"/>
+          <c:w val="0.74511206029922172"/>
+          <c:h val="0.80341956587858998"/>
         </c:manualLayout>
       </c:layout>
       <c:areaChart>
@@ -120,7 +129,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$31</c:f>
+              <c:f>Sheet1!$C$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -134,19 +143,19 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$31:$AV$31</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$30:$AV$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -159,8 +168,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="595469312"/>
-        <c:axId val="55640064"/>
+        <c:axId val="541138432"/>
+        <c:axId val="526963200"/>
       </c:areaChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -170,7 +179,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$32</c:f>
+              <c:f>Sheet1!$C$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -197,19 +206,19 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$32:$AV$32</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$31:$AV$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -220,43 +229,27 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$33</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700">
-              <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$33:$AV$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$C$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$32:$AV$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -267,41 +260,27 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$34</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700">
-              <a:solidFill>
-                <a:srgbClr val="00FFFF"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="00FFFF"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$34:$AV$34</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$C$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$33:$AV$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -312,27 +291,27 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$35</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$35:$AV$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$C$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$34:$AV$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -343,27 +322,27 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$36</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$36:$AV$36</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$C$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$35:$AV$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -374,27 +353,27 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$37</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$37:$AV$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$C$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$36:$AV$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -405,27 +384,27 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$38</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$38:$AV$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$C$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$37:$AV$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -436,27 +415,27 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$39</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$39:$AV$39</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$C$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$38:$AV$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -467,27 +446,27 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$40</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$40:$AV$40</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$C$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$39:$AV$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -498,27 +477,27 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$41</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$41:$AV$41</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$C$40</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$40:$AV$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -529,27 +508,27 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$42</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$42:$AV$42</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$C$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$41:$AV$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -560,27 +539,27 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$43</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$43:$AV$43</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$C$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$42:$AV$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -591,27 +570,27 @@
           <c:order val="13"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$44</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$44:$AV$44</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$C$43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$43:$AV$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -622,27 +601,213 @@
           <c:order val="14"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$45</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$45:$AV$45</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$C$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$44:$AV$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="15"/>
+          <c:order val="15"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$45:$AV$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="16"/>
+          <c:order val="16"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$46</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$46:$AV$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="17"/>
+          <c:order val="17"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$47</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$47:$AV$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="18"/>
+          <c:order val="18"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$48</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$48:$AV$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="19"/>
+          <c:order val="19"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$49:$AV$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="20"/>
+          <c:order val="20"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$50:$AV$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -658,42 +823,42 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="595469312"/>
-        <c:axId val="55640064"/>
+        <c:axId val="541138432"/>
+        <c:axId val="526963200"/>
       </c:lineChart>
-      <c:catAx>
-        <c:axId val="595469312"/>
+      <c:valAx>
+        <c:axId val="526963200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="541138432"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="541138432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55640064"/>
+        <c:crossAx val="526963200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
-      <c:valAx>
-        <c:axId val="55640064"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="#,##0.0;[Red]\-#,##0.0" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="595469312"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -701,10 +866,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.88132680122090457"/>
-          <c:y val="8.3496740672916198E-3"/>
-          <c:w val="0.11503541260115449"/>
-          <c:h val="0.9844366949690283"/>
+          <c:x val="0.85128636216833387"/>
+          <c:y val="3.9907939543454889E-2"/>
+          <c:w val="0.14160964714765939"/>
+          <c:h val="0.83926892348306981"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -744,7 +909,7 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -775,14 +940,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1093,10 +1258,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:S6"/>
+  <dimension ref="A3:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,73 +1269,53 @@
     <col min="1" max="1" width="3.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
+    <row r="3" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
+    <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
     </row>
-    <row r="6" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-    </row>
+    <row r="29" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A4:R4"/>
-    <mergeCell ref="A6:S6"/>
     <mergeCell ref="A5:S5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Combination Area Chart Excel Export logo change
</commit_message>
<xml_diff>
--- a/Merck Sereno Dashboard/Dashboard/Content/ExportTemplate/CombinationAreaChart.xlsx
+++ b/Merck Sereno Dashboard/Dashboard/Content/ExportTemplate/CombinationAreaChart.xlsx
@@ -15,7 +15,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -27,6 +27,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -64,7 +79,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -74,6 +89,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -117,8 +134,8 @@
           <c:yMode val="edge"/>
           <c:x val="5.0623120491736791E-2"/>
           <c:y val="6.6470669494486559E-2"/>
-          <c:w val="0.74511206029922172"/>
-          <c:h val="0.80341956587858998"/>
+          <c:w val="0.68387578069205823"/>
+          <c:h val="0.81288702267617419"/>
         </c:manualLayout>
       </c:layout>
       <c:areaChart>
@@ -168,8 +185,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="541138432"/>
-        <c:axId val="526963200"/>
+        <c:axId val="540097024"/>
+        <c:axId val="113168320"/>
       </c:areaChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -503,316 +520,6 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:ser>
-          <c:idx val="11"/>
-          <c:order val="11"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$41</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$D$29:$AV$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$41:$AV$41</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="12"/>
-          <c:order val="12"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$42</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$D$29:$AV$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$42:$AV$42</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="13"/>
-          <c:order val="13"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$43</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$D$29:$AV$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$43:$AV$43</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="14"/>
-          <c:order val="14"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$44</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$D$29:$AV$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$44:$AV$44</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="15"/>
-          <c:order val="15"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$45</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$D$29:$AV$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$45:$AV$45</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="16"/>
-          <c:order val="16"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$46</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$D$29:$AV$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$46:$AV$46</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="17"/>
-          <c:order val="17"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$47</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$D$29:$AV$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$47:$AV$47</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="18"/>
-          <c:order val="18"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$48</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$D$29:$AV$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$48:$AV$48</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="19"/>
-          <c:order val="19"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$49</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$D$29:$AV$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$49:$AV$49</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="20"/>
-          <c:order val="20"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$50</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$D$29:$AV$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$50:$AV$50</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -823,11 +530,44 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="541138432"/>
-        <c:axId val="526963200"/>
+        <c:axId val="540098048"/>
+        <c:axId val="113168896"/>
       </c:lineChart>
+      <c:catAx>
+        <c:axId val="540097024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="113168320"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="526963200"/>
+        <c:axId val="113168320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="#,##0.0;[Red]\-#,##0.0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="540097024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="113168896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -837,12 +577,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541138432"/>
+        <c:crossAx val="540098048"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="541138432"/>
+        <c:axId val="540098048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -852,7 +592,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="526963200"/>
+        <c:crossAx val="113168896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -866,10 +606,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.85128636216833387"/>
-          <c:y val="3.9907939543454889E-2"/>
-          <c:w val="0.14160964714765939"/>
-          <c:h val="0.83926892348306981"/>
+          <c:x val="0.79698249157330203"/>
+          <c:y val="2.7284663813342554E-2"/>
+          <c:w val="0.19591351774269117"/>
+          <c:h val="0.9465667671890251"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1260,13 +1000,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1312,7 +1052,9 @@
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
     </row>
-    <row r="29" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A4:R4"/>

</xml_diff>

<commit_message>
Market Share Excel Export Working on export for MAT and YTD Special
</commit_message>
<xml_diff>
--- a/Merck Sereno Dashboard/Dashboard/Content/ExportTemplate/CombinationAreaChart.xlsx
+++ b/Merck Sereno Dashboard/Dashboard/Content/ExportTemplate/CombinationAreaChart.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621" calcMode="manual"/>
 </workbook>
@@ -83,14 +84,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -185,8 +186,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="540097024"/>
-        <c:axId val="113168320"/>
+        <c:axId val="541674496"/>
+        <c:axId val="120640000"/>
       </c:areaChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -530,11 +531,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="540098048"/>
-        <c:axId val="113168896"/>
+        <c:axId val="570974208"/>
+        <c:axId val="120640576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="540097024"/>
+        <c:axId val="541674496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -544,7 +545,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113168320"/>
+        <c:crossAx val="120640000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -552,7 +553,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113168320"/>
+        <c:axId val="120640000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -562,12 +563,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="540097024"/>
+        <c:crossAx val="541674496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="113168896"/>
+        <c:axId val="120640576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -577,12 +578,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="540098048"/>
+        <c:crossAx val="570974208"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="540098048"/>
+        <c:axId val="570974208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -592,7 +593,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113168896"/>
+        <c:crossAx val="120640576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -609,6 +610,203 @@
           <c:x val="0.79698249157330203"/>
           <c:y val="2.7284663813342554E-2"/>
           <c:w val="0.19591351774269117"/>
+          <c:h val="0.9465667671890251"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.0623120491736791E-2"/>
+          <c:y val="6.6470669494486559E-2"/>
+          <c:w val="0.68387578069205823"/>
+          <c:h val="0.81288702267617419"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$C$30:$C$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$30:$D$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$E$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="000080"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$C$30:$C$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$E$30:$E$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="570976256"/>
+        <c:axId val="571032704"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="570976256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="571032704"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="571032704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="#,##0.0;[Red]\-#,##0.0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="570976256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.88248220272292655"/>
+          <c:y val="2.7284663813342554E-2"/>
+          <c:w val="0.11041380659306668"/>
           <c:h val="0.9465667671890251"/>
         </c:manualLayout>
       </c:layout>
@@ -692,6 +890,81 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="11182350" cy="685799"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart1"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1000,60 +1273,130 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
     </row>
     <row r="29" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
+      <c r="A29" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A4:R4"/>
+    <mergeCell ref="A5:S5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:S29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.140625" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="1"/>
+    </row>
+    <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+    </row>
+    <row r="29" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>